<commit_message>
Add usedRange to Sheet.
</commit_message>
<xml_diff>
--- a/examples/shared-formulas/out.xlsx
+++ b/examples/shared-formulas/out.xlsx
@@ -1713,8 +1713,12 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
+      <c r="B1"/>
+      <c r="C1"/>
+      <c r="D1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1726,121 +1730,132 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3"/>
       <c r="B3" s="1">
-        <v>812</v>
+        <v>509</v>
       </c>
       <c r="C3" s="1">
-        <v>17596</v>
+        <v>346380</v>
       </c>
       <c r="D3" s="5">
         <f t="shared" si="1" ref="D3:D13">B3/C3</f>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4"/>
       <c r="B4" s="1">
-        <v>380</v>
+        <v>614</v>
       </c>
       <c r="C4" s="1">
-        <v>621352</v>
+        <v>293935</v>
       </c>
       <c r="D4" s="6">
         <f t="shared" si="1"/>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5"/>
       <c r="B5" s="1">
-        <v>395</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1">
-        <v>814325</v>
+        <v>899517</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="1"/>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6"/>
       <c r="B6">
-        <v>606</v>
+        <v>617</v>
       </c>
       <c r="C6" s="1">
-        <v>332744</v>
+        <v>781247</v>
       </c>
       <c r="D6" s="8">
         <f t="shared" si="1"/>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7"/>
       <c r="B7" s="1">
-        <v>49</v>
+        <v>975</v>
       </c>
       <c r="C7" s="1">
-        <v>815717</v>
+        <v>800261</v>
       </c>
       <c r="D7" s="9">
         <f t="shared" si="1"/>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8"/>
       <c r="B8">
-        <v>371</v>
+        <v>99</v>
       </c>
       <c r="C8" s="1">
-        <v>781845</v>
+        <v>333038</v>
       </c>
       <c r="D8" s="10">
         <f t="shared" si="1"/>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9"/>
       <c r="B9">
-        <v>393</v>
+        <v>810</v>
       </c>
       <c r="C9" s="1">
-        <v>569500</v>
+        <v>843502</v>
       </c>
       <c r="D9" s="11">
         <f t="shared" si="1"/>
       </c>
     </row>
     <row r="10">
+      <c r="A10"/>
       <c r="B10">
-        <v>238</v>
+        <v>976</v>
       </c>
       <c r="C10">
-        <v>319935</v>
+        <v>132730</v>
       </c>
       <c r="D10" s="12">
         <f t="shared" si="1"/>
       </c>
     </row>
     <row r="11">
+      <c r="A11"/>
       <c r="B11">
-        <v>702</v>
+        <v>214</v>
       </c>
       <c r="C11">
-        <v>678651</v>
+        <v>57169</v>
       </c>
       <c r="D11" s="13">
         <f t="shared" si="1"/>
       </c>
     </row>
     <row r="12">
+      <c r="A12"/>
       <c r="B12">
-        <v>526</v>
+        <v>961</v>
       </c>
       <c r="C12">
-        <v>751536</v>
+        <v>717649</v>
       </c>
       <c r="D12" s="14">
         <f t="shared" si="1"/>
       </c>
     </row>
     <row r="13">
+      <c r="A13"/>
       <c r="B13">
-        <v>58</v>
+        <v>880</v>
       </c>
       <c r="C13">
-        <v>655140</v>
+        <v>32781</v>
       </c>
       <c r="D13" s="15">
         <f t="shared" si="1"/>

</xml_diff>